<commit_message>
Get RFECV features and update best features so far
</commit_message>
<xml_diff>
--- a/playground_4.6/model_tracker_p_4.6.xlsx
+++ b/playground_4.6/model_tracker_p_4.6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adeniyi Babalola\Documents\GitHub\kaggle\kaggle_competition\playground_4.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC7098C-A2F4-40C1-858E-B8203718ED5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08DA83C-50DD-4D86-9476-708E7AFDF7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="preprocess 3cv" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'preprocess 3cv'!$A$2:$G$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'preprocess 3cv'!$A$2:$H$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Permutation Imp</t>
+  </si>
+  <si>
+    <t>RFECV</t>
   </si>
 </sst>
 </file>
@@ -691,7 +694,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -727,7 +730,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1215,11 +1217,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D12" sqref="D12"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1227,18 +1229,18 @@
     <col min="1" max="1" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="6" width="16.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>13</v>
       </c>
@@ -1246,8 +1248,9 @@
       <c r="C1" s="22"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1263,11 +1266,14 @@
       <c r="E2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1283,15 +1289,18 @@
       <c r="E3" s="18">
         <v>0.83136818702441895</v>
       </c>
-      <c r="F3" s="8">
-        <f>(C3-E3)/C3</f>
-        <v>5.4114203220859331E-4</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="18">
+        <v>0.83181831887992597</v>
+      </c>
+      <c r="G3" s="8">
+        <f>(C3-F3)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1307,22 +1316,25 @@
       <c r="E4" s="19">
         <v>0.82111630802387703</v>
       </c>
-      <c r="F4" s="8">
-        <f>(C4-E4)/C4</f>
-        <v>1.3246555544068677E-3</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="19">
+        <v>0.82280078632111897</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" ref="G4:G12" si="0">(C4-F4)/C4</f>
+        <v>-7.2407606530455759E-4</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="19">
         <v>0.76538516395599998</v>
       </c>
       <c r="D5" s="18">
@@ -1331,13 +1343,16 @@
       <c r="E5" s="18">
         <v>0.77658077210971399</v>
       </c>
-      <c r="F5" s="8">
-        <f t="shared" ref="F5:F12" si="0">(C5-E5)/C5</f>
+      <c r="F5" s="18">
+        <v>0.77658077210971399</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
         <v>-1.4627417254664236E-2</v>
       </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1353,15 +1368,18 @@
       <c r="E6" s="19">
         <v>0.83051139508148997</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="19">
+        <v>0.83059851574360699</v>
+      </c>
+      <c r="G6" s="8">
         <f t="shared" si="0"/>
-        <v>-1.5737225345440468E-4</v>
-      </c>
-      <c r="G6" s="12" t="s">
+        <v>-2.6228878200293122E-4</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1377,15 +1395,18 @@
       <c r="E7" s="19">
         <v>0.79872511912879596</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="19">
+        <v>0.79872511912879596</v>
+      </c>
+      <c r="G7" s="8">
         <f t="shared" si="0"/>
         <v>-6.1276159243883977E-3</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1401,15 +1422,18 @@
       <c r="E8" s="19">
         <v>0.83091793497630495</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="19">
+        <v>0.83091793497630495</v>
+      </c>
+      <c r="G8" s="8">
         <f t="shared" si="0"/>
         <v>-9.0952279343710807E-4</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1425,15 +1449,18 @@
       <c r="E9" s="19">
         <v>0.737722700558338</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="19">
+        <v>0.80210837864348505</v>
+      </c>
+      <c r="G9" s="8">
         <f t="shared" si="0"/>
-        <v>-9.1171610496952361E-3</v>
-      </c>
-      <c r="G9" s="7" t="s">
+        <v>-9.7189132580961998E-2</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1449,12 +1476,15 @@
       <c r="E10" s="19">
         <v>0.81670197939510703</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="19">
+        <v>0.81670199837288704</v>
+      </c>
+      <c r="G10" s="8">
         <f t="shared" si="0"/>
-        <v>2.3237092662867657E-8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1470,12 +1500,15 @@
       <c r="E11" s="19">
         <v>0.82447071076973399</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="19">
+        <v>0.82564679542682695</v>
+      </c>
+      <c r="G11" s="8">
         <f t="shared" si="0"/>
-        <v>-3.3478041121893311E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-1.7617302977706523E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1491,15 +1524,18 @@
       <c r="E12" s="18">
         <v>0.82988697551162005</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="18">
+        <v>0.82978529889223296</v>
+      </c>
+      <c r="G12" s="8">
         <f t="shared" si="0"/>
-        <v>6.9936258413655892E-4</v>
-      </c>
-      <c r="G12" s="14" t="s">
+        <v>8.2179553411890096E-4</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1508,12 +1544,13 @@
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1524,12 +1561,13 @@
         <v>35</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="20" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1537,8 +1575,9 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>14</v>
       </c>
@@ -1546,8 +1585,9 @@
       <c r="C17" s="21"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>11</v>
       </c>
@@ -1555,8 +1595,9 @@
       <c r="C18" s="21"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>30</v>
       </c>
@@ -1564,20 +1605,23 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C12">
@@ -1589,38 +1633,38 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A17:C17"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:E3">
+  <conditionalFormatting sqref="C3:F3">
     <cfRule type="top10" dxfId="10" priority="43" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:E12">
+  <conditionalFormatting sqref="C3:F12">
     <cfRule type="top10" dxfId="9" priority="45" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:E5">
+  <conditionalFormatting sqref="C4:F5">
     <cfRule type="top10" dxfId="8" priority="47" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E6">
-    <cfRule type="top10" dxfId="7" priority="49" rank="1"/>
+  <conditionalFormatting sqref="C5:F5">
+    <cfRule type="top10" dxfId="7" priority="63" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:E7">
-    <cfRule type="top10" dxfId="6" priority="51" rank="1"/>
+  <conditionalFormatting sqref="C6:F6">
+    <cfRule type="top10" dxfId="6" priority="49" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:E8">
-    <cfRule type="top10" dxfId="5" priority="53" rank="1"/>
+  <conditionalFormatting sqref="C7:F7">
+    <cfRule type="top10" dxfId="5" priority="51" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:E9">
-    <cfRule type="top10" dxfId="4" priority="55" rank="1"/>
+  <conditionalFormatting sqref="C8:F8">
+    <cfRule type="top10" dxfId="4" priority="53" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:E10">
-    <cfRule type="top10" dxfId="3" priority="57" rank="1"/>
+  <conditionalFormatting sqref="C9:F9">
+    <cfRule type="top10" dxfId="3" priority="55" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:E11">
-    <cfRule type="top10" dxfId="2" priority="59" rank="1"/>
+  <conditionalFormatting sqref="C10:F10">
+    <cfRule type="top10" dxfId="2" priority="57" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:E12">
-    <cfRule type="top10" dxfId="1" priority="61" rank="1"/>
+  <conditionalFormatting sqref="C11:F11">
+    <cfRule type="top10" dxfId="1" priority="59" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:E5">
-    <cfRule type="top10" dxfId="0" priority="63" rank="1"/>
+  <conditionalFormatting sqref="C12:F12">
+    <cfRule type="top10" dxfId="0" priority="61" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>